<commit_message>
adding kmeans ml library
</commit_message>
<xml_diff>
--- a/programs/frameworks/neural/data/km.xlsx
+++ b/programs/frameworks/neural/data/km.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\objec\Documents\Code\objeck-lang\programs\frameworks\neural\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD6C3B0-BA72-4337-99CD-BC6202121EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7EDC19-9E82-44D2-B945-8262352BC5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="1310" windowWidth="21560" windowHeight="12550" activeTab="1" xr2:uid="{0A150D75-2C26-4F3F-A19F-9DE0B9471383}"/>
+    <workbookView xWindow="400" yWindow="780" windowWidth="19890" windowHeight="14240" activeTab="1" xr2:uid="{0A150D75-2C26-4F3F-A19F-9DE0B9471383}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="2" r:id="rId1"/>
@@ -135,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -145,7 +145,6 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -780,13 +779,6 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:noFill/>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-48B3-4B40-8022-F609E9F77A44}"/>
@@ -839,10 +831,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Model (2)'!$B$1:$P$1</c:f>
+              <c:f>'Model (2)'!$B$1:$O$1</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>9.7840100000000003</c:v>
                 </c:pt>
@@ -880,23 +872,20 @@
                   <c:v>0.54972600000000005</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>1.64</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.25</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5</c:v>
+                  <c:v>7.8319999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Model (2)'!$B$2:$P$2</c:f>
+              <c:f>'Model (2)'!$B$2:$O$2</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>7.8598999999999997</c:v>
                 </c:pt>
@@ -934,13 +923,10 @@
                   <c:v>6.2730920000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6</c:v>
+                  <c:v>2.6585709999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.75</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5</c:v>
+                  <c:v>6.63</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2301,16 +2287,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>3175</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>149225</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2695,7 +2681,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="7">
@@ -2734,10 +2720,10 @@
       <c r="M1" s="7">
         <v>0.54972600000000005</v>
       </c>
-      <c r="N1" s="10">
+      <c r="N1" s="9">
         <v>4</v>
       </c>
-      <c r="O1" s="10">
+      <c r="O1" s="9">
         <v>7.25</v>
       </c>
       <c r="P1" s="8">
@@ -2748,7 +2734,7 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="7">
@@ -2787,10 +2773,10 @@
       <c r="M2" s="7">
         <v>6.2730920000000001</v>
       </c>
-      <c r="N2" s="10">
+      <c r="N2" s="9">
         <v>6</v>
       </c>
-      <c r="O2" s="10">
+      <c r="O2" s="9">
         <v>6.75</v>
       </c>
       <c r="P2" s="8">
@@ -2866,51 +2852,51 @@
         <v>1</v>
       </c>
       <c r="B5" s="3">
-        <f>SQRT(POWER(B1-$O$1, 2)+POWER(B2-$O$2, 2))</f>
+        <f t="shared" ref="B5:M5" si="1">SQRT(POWER(B1-$O$1, 2)+POWER(B2-$O$2, 2))</f>
         <v>2.7664209170153411</v>
       </c>
       <c r="C5" s="3">
-        <f>SQRT(POWER(C1-$O$1, 2)+POWER(C2-$O$2, 2))</f>
+        <f t="shared" si="1"/>
         <v>8.7866187545073338</v>
       </c>
       <c r="D5" s="3">
-        <f>SQRT(POWER(D1-$O$1, 2)+POWER(D2-$O$2, 2))</f>
+        <f t="shared" si="1"/>
         <v>2.0219263999463486</v>
       </c>
       <c r="E5" s="3">
-        <f>SQRT(POWER(E1-$O$1, 2)+POWER(E2-$O$2, 2))</f>
+        <f t="shared" si="1"/>
         <v>8.3464655459633939</v>
       </c>
       <c r="F5" s="3">
-        <f>SQRT(POWER(F1-$O$1, 2)+POWER(F2-$O$2, 2))</f>
+        <f t="shared" si="1"/>
         <v>1.1031394211975198</v>
       </c>
       <c r="G5" s="3">
-        <f>SQRT(POWER(G1-$O$1, 2)+POWER(G2-$O$2, 2))</f>
+        <f t="shared" si="1"/>
         <v>2.1075714097116616</v>
       </c>
       <c r="H5" s="3">
-        <f>SQRT(POWER(H1-$O$1, 2)+POWER(H2-$O$2, 2))</f>
+        <f t="shared" si="1"/>
         <v>7.4408104015960523</v>
       </c>
       <c r="I5" s="3">
-        <f>SQRT(POWER(I1-$O$1, 2)+POWER(I2-$O$2, 2))</f>
+        <f t="shared" si="1"/>
         <v>2.3464515012897667</v>
       </c>
       <c r="J5" s="3">
-        <f>SQRT(POWER(J1-$O$1, 2)+POWER(J2-$O$2, 2))</f>
+        <f t="shared" si="1"/>
         <v>5.4994124611725566</v>
       </c>
       <c r="K5" s="3">
-        <f>SQRT(POWER(K1-$O$1, 2)+POWER(K2-$O$2, 2))</f>
+        <f t="shared" si="1"/>
         <v>7.0681219801546291</v>
       </c>
       <c r="L5" s="3">
-        <f>SQRT(POWER(L1-$O$1, 2)+POWER(L2-$O$2, 2))</f>
+        <f t="shared" si="1"/>
         <v>6.5032301864227442</v>
       </c>
       <c r="M5" s="3">
-        <f>SQRT(POWER(M1-$O$1, 2)+POWER(M2-$O$2, 2))</f>
+        <f t="shared" si="1"/>
         <v>6.7172250904328052</v>
       </c>
       <c r="N5" s="1"/>
@@ -2927,47 +2913,47 @@
         <v>k2</v>
       </c>
       <c r="C6" s="4" t="str">
-        <f t="shared" ref="C6:M6" si="1">IF(MIN(C4:C5)=C4,"k1","k2")</f>
+        <f t="shared" ref="C6:M6" si="2">IF(MIN(C4:C5)=C4,"k1","k2")</f>
         <v>k1</v>
       </c>
       <c r="D6" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>k2</v>
       </c>
       <c r="E6" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>k1</v>
       </c>
       <c r="F6" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>k2</v>
       </c>
       <c r="G6" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>k2</v>
       </c>
       <c r="H6" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>k1</v>
       </c>
       <c r="I6" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>k2</v>
       </c>
       <c r="J6" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>k1</v>
       </c>
       <c r="K6" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>k1</v>
       </c>
       <c r="L6" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>k1</v>
       </c>
       <c r="M6" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>k1</v>
       </c>
       <c r="N6" s="1"/>
@@ -2984,47 +2970,47 @@
         <v>9.6632666446880684</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" ref="C8:M8" si="2">SQRT(POWER(C1-$P$1, 2)+POWER(C2-$P$2, 2))</f>
+        <f t="shared" ref="C8:M8" si="3">SQRT(POWER(C1-$P$1, 2)+POWER(C2-$P$2, 2))</f>
         <v>2.0598759718966089</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.7196316066170558</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.237475798614367</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.9953950974010883</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.7754520248696153</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.54840870162771838</v>
       </c>
       <c r="I8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.5149309855684585</v>
       </c>
       <c r="J8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.7072766455267292</v>
       </c>
       <c r="K8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.6042320749548677</v>
       </c>
       <c r="L8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.7916205806032146</v>
       </c>
       <c r="M8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.7753754057731799</v>
       </c>
     </row>
@@ -3037,47 +3023,47 @@
         <v>2.3071621204631461</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" ref="C9:M9" si="3">SQRT(POWER(C1-$Q$1, 2)+POWER(C2-$Q$2, 2))</f>
+        <f t="shared" ref="C9:M9" si="4">SQRT(POWER(C1-$Q$1, 2)+POWER(C2-$Q$2, 2))</f>
         <v>9.1444665275269053</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.5178508117730152</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.6510550617802675</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.6752636277911599</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.4764999711354734</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.865853654403951</v>
       </c>
       <c r="I9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.1379213437133271</v>
       </c>
       <c r="J9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.8508127485076811</v>
       </c>
       <c r="K9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.5645487607883792</v>
       </c>
       <c r="L9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.7971767299077932</v>
       </c>
       <c r="M9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.2910148766505749</v>
       </c>
     </row>
@@ -3090,47 +3076,47 @@
         <v>k2</v>
       </c>
       <c r="C10" s="4" t="str">
-        <f t="shared" ref="C10:M10" si="4">IF(MIN(C8:C9)=C8,"k1","k2")</f>
+        <f t="shared" ref="C10:M10" si="5">IF(MIN(C8:C9)=C8,"k1","k2")</f>
         <v>k1</v>
       </c>
       <c r="D10" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>k2</v>
       </c>
       <c r="E10" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>k1</v>
       </c>
       <c r="F10" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>k2</v>
       </c>
       <c r="G10" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>k2</v>
       </c>
       <c r="H10" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>k1</v>
       </c>
       <c r="I10" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>k2</v>
       </c>
       <c r="J10" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>k1</v>
       </c>
       <c r="K10" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>k1</v>
       </c>
       <c r="L10" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>k1</v>
       </c>
       <c r="M10" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>k1</v>
       </c>
     </row>
@@ -3144,8 +3130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B524A5-C02E-46BA-855D-C1583E2922D2}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3154,7 +3140,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="7">
@@ -3194,17 +3180,17 @@
         <v>0.54972600000000005</v>
       </c>
       <c r="N1" s="3">
-        <v>4</v>
+        <v>1.64</v>
       </c>
       <c r="O1" s="3">
-        <v>7.25</v>
+        <v>7.8319999999999999</v>
       </c>
       <c r="P1" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="7">
@@ -3244,10 +3230,10 @@
         <v>6.2730920000000001</v>
       </c>
       <c r="N2" s="3">
-        <v>6</v>
+        <v>2.6585709999999998</v>
       </c>
       <c r="O2" s="3">
-        <v>6.75</v>
+        <v>6.63</v>
       </c>
       <c r="P2" s="3">
         <v>5</v>

</xml_diff>